<commit_message>
chapter 5 example 3
</commit_message>
<xml_diff>
--- a/src/Chapter-5/02/采购表/1.xlsx
+++ b/src/Chapter-5/02/采购表/1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MGF\Documents\GitHub\TianXiaPy\PyExcel\src\Chapter-5\02\采购表\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F5E4B5-8A14-4245-8EF6-AD792FCE8F73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC42E646-424C-4DBC-9383-7D3CC03B1BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="采购" sheetId="1" r:id="rId1"/>

</xml_diff>